<commit_message>
Fix rules (replace None and Goal with 0 and 100)
</commit_message>
<xml_diff>
--- a/wherearethecows.xlsx
+++ b/wherearethecows.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hrnl-my.sharepoint.com/personal/bootb_hr_nl/Documents/Bureaublad/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bas/Code/Python/Cows/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2309F8F2-65ED-A344-9DB4-98D74A3BA9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732DF96C-CADF-C746-AB4B-4473067D3697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{BAF0BDC9-5433-4F74-93BD-B5CA7F73E396}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" xr2:uid="{BAF0BDC9-5433-4F74-93BD-B5CA7F73E396}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="46">
   <si>
     <t>Opmerking</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Zwart</t>
   </si>
   <si>
-    <t>GOAL</t>
-  </si>
-  <si>
-    <t>EINDE</t>
-  </si>
-  <si>
     <t>START pion1</t>
   </si>
   <si>
@@ -177,6 +171,9 @@
   </si>
   <si>
     <t>lugnut</t>
+  </si>
+  <si>
+    <t>EINDE, nummer 100 noodzakelijk om te zorgen dat het allemaal getallen zijn -&gt; let op dat dit geen echt nummer is, dus de getalvragen op False moeten. Ook 0 bestaat niet = None</t>
   </si>
 </sst>
 </file>
@@ -573,7 +570,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -583,58 +580,58 @@
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -650,44 +647,44 @@
       <c r="E2">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>27</v>
-      </c>
-      <c r="R2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -703,41 +700,41 @@
       <c r="E3">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>27</v>
-      </c>
       <c r="R3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -753,41 +750,41 @@
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" t="s">
-        <v>14</v>
-      </c>
-      <c r="N4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>27</v>
-      </c>
       <c r="R4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -795,7 +792,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>26</v>
@@ -803,44 +800,44 @@
       <c r="E5">
         <v>5</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O5" t="s">
+        <v>11</v>
+      </c>
+      <c r="P5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" t="s">
         <v>25</v>
       </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" t="s">
-        <v>13</v>
-      </c>
-      <c r="M5" t="s">
-        <v>13</v>
-      </c>
-      <c r="N5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O5" t="s">
-        <v>13</v>
-      </c>
-      <c r="P5" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>27</v>
-      </c>
       <c r="R5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -848,7 +845,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -856,44 +853,44 @@
       <c r="E6">
         <v>35</v>
       </c>
-      <c r="F6" t="s">
-        <v>25</v>
+      <c r="F6">
+        <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="M6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="N6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="O6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="P6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
@@ -909,41 +906,41 @@
       <c r="E7">
         <v>40</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7" t="s">
+        <v>12</v>
+      </c>
+      <c r="O7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q7" t="s">
         <v>25</v>
       </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" t="s">
-        <v>13</v>
-      </c>
-      <c r="M7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O7" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>27</v>
-      </c>
       <c r="R7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -951,7 +948,7 @@
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -959,41 +956,41 @@
       <c r="E8">
         <v>50</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" t="s">
+        <v>11</v>
+      </c>
+      <c r="O8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q8" t="s">
         <v>25</v>
       </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" t="s">
-        <v>14</v>
-      </c>
-      <c r="M8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N8" t="s">
-        <v>13</v>
-      </c>
-      <c r="O8" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>27</v>
-      </c>
-      <c r="R8" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
@@ -1001,7 +998,7 @@
         <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <v>61</v>
@@ -1009,44 +1006,44 @@
       <c r="E9">
         <v>55</v>
       </c>
-      <c r="F9" t="s">
-        <v>25</v>
+      <c r="F9">
+        <v>0</v>
       </c>
       <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P9" t="s">
         <v>14</v>
       </c>
-      <c r="H9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M9" t="s">
-        <v>13</v>
-      </c>
-      <c r="N9" t="s">
-        <v>13</v>
-      </c>
-      <c r="O9" t="s">
-        <v>13</v>
-      </c>
-      <c r="P9" t="s">
-        <v>16</v>
-      </c>
       <c r="Q9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -1062,41 +1059,41 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q10" t="s">
         <v>25</v>
       </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" t="s">
-        <v>13</v>
-      </c>
-      <c r="K10" t="s">
-        <v>13</v>
-      </c>
-      <c r="L10" t="s">
-        <v>13</v>
-      </c>
-      <c r="M10" t="s">
-        <v>13</v>
-      </c>
-      <c r="N10" t="s">
-        <v>13</v>
-      </c>
-      <c r="O10" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>27</v>
-      </c>
       <c r="R10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -1104,7 +1101,7 @@
         <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <v>65</v>
@@ -1112,44 +1109,44 @@
       <c r="E11">
         <v>60</v>
       </c>
-      <c r="F11" t="s">
-        <v>25</v>
+      <c r="F11">
+        <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="N11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="O11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="P11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="Q11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="R11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -1157,49 +1154,49 @@
         <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="D12" s="1">
+        <v>100</v>
       </c>
       <c r="E12">
         <v>26</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O12" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q12" t="s">
         <v>25</v>
       </c>
-      <c r="G12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" t="s">
-        <v>13</v>
-      </c>
-      <c r="L12" t="s">
-        <v>13</v>
-      </c>
-      <c r="M12" t="s">
-        <v>13</v>
-      </c>
-      <c r="N12" t="s">
-        <v>13</v>
-      </c>
-      <c r="O12" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>27</v>
-      </c>
       <c r="R12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -1212,47 +1209,47 @@
       <c r="D13">
         <v>15</v>
       </c>
-      <c r="E13" t="s">
-        <v>25</v>
+      <c r="E13">
+        <v>0</v>
       </c>
       <c r="F13" s="1">
         <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="M13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="N13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="O13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="P13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Q13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -1260,52 +1257,52 @@
         <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D14">
         <v>25</v>
       </c>
-      <c r="E14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" t="s">
-        <v>25</v>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="M14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="N14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="O14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="P14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -1313,52 +1310,52 @@
         <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" t="s">
-        <v>25</v>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" t="s">
+        <v>11</v>
+      </c>
+      <c r="N15" t="s">
+        <v>11</v>
+      </c>
+      <c r="O15" t="s">
+        <v>11</v>
+      </c>
+      <c r="P15" t="s">
         <v>13</v>
       </c>
-      <c r="I15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K15" t="s">
-        <v>13</v>
-      </c>
-      <c r="L15" t="s">
-        <v>13</v>
-      </c>
-      <c r="M15" t="s">
-        <v>13</v>
-      </c>
-      <c r="N15" t="s">
-        <v>13</v>
-      </c>
-      <c r="O15" t="s">
-        <v>13</v>
-      </c>
-      <c r="P15" t="s">
-        <v>15</v>
-      </c>
       <c r="Q15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -1371,47 +1368,47 @@
       <c r="D16">
         <v>75</v>
       </c>
-      <c r="E16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" t="s">
-        <v>25</v>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="M16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="N16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="O16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="P16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Q16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
@@ -1427,94 +1424,94 @@
       <c r="E17">
         <v>50</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17" t="s">
+        <v>11</v>
+      </c>
+      <c r="M17" t="s">
+        <v>11</v>
+      </c>
+      <c r="N17" t="s">
+        <v>11</v>
+      </c>
+      <c r="O17" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q17" t="s">
         <v>25</v>
       </c>
-      <c r="G17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" t="s">
-        <v>13</v>
-      </c>
-      <c r="J17" t="s">
-        <v>13</v>
-      </c>
-      <c r="K17" t="s">
-        <v>13</v>
-      </c>
-      <c r="L17" t="s">
-        <v>13</v>
-      </c>
-      <c r="M17" t="s">
-        <v>13</v>
-      </c>
-      <c r="N17" t="s">
-        <v>13</v>
-      </c>
-      <c r="O17" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>27</v>
-      </c>
       <c r="R17" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>2</v>
+      <c r="A18" s="1">
+        <v>100</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
       </c>
-      <c r="D18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" t="s">
-        <v>25</v>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="M18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="N18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="O18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="P18" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="Q18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R18" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix is_red, is_green, is_odd, is_multiple5
</commit_message>
<xml_diff>
--- a/wherearethecows.xlsx
+++ b/wherearethecows.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bas/Code/Python/Cows/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732DF96C-CADF-C746-AB4B-4473067D3697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF298AE1-6788-BC46-8D58-0C8807198932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" xr2:uid="{BAF0BDC9-5433-4F74-93BD-B5CA7F73E396}"/>
   </bookViews>
@@ -570,7 +570,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -666,10 +666,10 @@
         <v>12</v>
       </c>
       <c r="L2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N2" t="s">
         <v>11</v>
@@ -719,7 +719,7 @@
         <v>11</v>
       </c>
       <c r="L3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M3" t="s">
         <v>11</v>
@@ -769,16 +769,16 @@
         <v>12</v>
       </c>
       <c r="L4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q4" t="s">
         <v>25</v>
@@ -822,7 +822,7 @@
         <v>11</v>
       </c>
       <c r="M5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N5" t="s">
         <v>12</v>
@@ -875,10 +875,10 @@
         <v>11</v>
       </c>
       <c r="M6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O6" t="s">
         <v>11</v>
@@ -975,16 +975,16 @@
         <v>12</v>
       </c>
       <c r="L8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M8" t="s">
         <v>12</v>
       </c>
       <c r="N8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q8" t="s">
         <v>25</v>
@@ -1028,7 +1028,7 @@
         <v>11</v>
       </c>
       <c r="M9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N9" t="s">
         <v>11</v>
@@ -1084,10 +1084,10 @@
         <v>11</v>
       </c>
       <c r="N10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q10" t="s">
         <v>25</v>
@@ -1128,16 +1128,16 @@
         <v>11</v>
       </c>
       <c r="L11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N11" t="s">
         <v>11</v>
       </c>
       <c r="O11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P11" t="s">
         <v>5</v>
@@ -1184,13 +1184,13 @@
         <v>11</v>
       </c>
       <c r="M12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N12" t="s">
         <v>11</v>
       </c>
       <c r="O12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q12" t="s">
         <v>25</v>
@@ -1237,10 +1237,10 @@
         <v>11</v>
       </c>
       <c r="N13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P13" t="s">
         <v>8</v>
@@ -1284,7 +1284,7 @@
         <v>12</v>
       </c>
       <c r="L14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M14" t="s">
         <v>11</v>
@@ -1293,7 +1293,7 @@
         <v>11</v>
       </c>
       <c r="O14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P14" t="s">
         <v>7</v>
@@ -1340,10 +1340,10 @@
         <v>11</v>
       </c>
       <c r="M15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O15" t="s">
         <v>11</v>
@@ -1396,10 +1396,10 @@
         <v>11</v>
       </c>
       <c r="N16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P16" t="s">
         <v>9</v>
@@ -1449,10 +1449,10 @@
         <v>11</v>
       </c>
       <c r="N17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q17" t="s">
         <v>25</v>

</xml_diff>